<commit_message>
update while cleaning laptop
</commit_message>
<xml_diff>
--- a/Wes/figure/Database.xlsx
+++ b/Wes/figure/Database.xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bubbl\OneDrive\Desktop\Summer2018\Wes\figure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bubbl\OneDrive\Desktop\SUM2018\Wes\figure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9A95B9D-0B98-4D2B-86D7-B6853B8DAAE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38C0778F-2116-488A-A410-BA6D3BA1ABCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25020" yWindow="200" windowWidth="25600" windowHeight="24900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1818,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G65" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>